<commit_message>
edge new 3  commit
</commit_message>
<xml_diff>
--- a/GII.xlsx
+++ b/GII.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,23 +539,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Insulin Pump Market Size, Share, Growth Analysis, By Type (Patch Pumps, And Tethered Pumps), By Product (MiniMed, Accu-Chek), By Accessories (Insulin Reservoir or Cartridges, Insulin Set Insertion Devices), By End Use (Hospitals &amp; Clinics, Homecare), By Region - Industry Forecast 2024-2031</t>
+          <t>Propolis Market Size, Share, Growth Analysis, By Product Type (Capsules and Tablets, Liquids), By Distribution Channel (Retail Store, Online), By Region - Industry Forecast 2024-2031</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SQMIG35A2135</t>
+          <t>SQMIG35A2163</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.skyquestt.com/report/insulin-pump-market</t>
+          <t>https://www.skyquestt.com/report/propolis-market</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>157</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -576,20 +576,361 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
+          <t>Global Propolis Market size was valued at USD 651.57 million in 2022 and is poised to grow from USD 666.69 million in 2023 to USD 800.96 million by 2031, growing at a CAGR of 2.32% during the forecast period (2024-2031).
+The global propolis market is experiencing robust growth driven by increasing consumer demand for natural health products, leveraging its rich composition of flavonoids, phenolic acids, and terpenes known for their antimicrobial, anti-inflammatory, and antioxidant properties. Propolis has proven effective in addressing various health issues, including colds, sore throats, dental cavities, and skin injuries, although potential allergic reactions necessitate cautious use. Its versatility results in widespread applications across food and beverages, pharmaceuticals, and cosmetics, further amplifying its market appeal. As health consciousness rises, consumers are increasingly prioritizing natural products, propelling market expansion. Key players predominantly hail from Brazil, China, and Europe, where a mix of large, established companies and numerous small-scale producers create a fragmented market landscape. North America is poised to take the lead in market share, fueled by the rising demand for natural and organic offerings. Meanwhile, the Asia-Pacific region is expected to experience the fastest growth rate, driven by heightened awareness regarding propolis's health benefits, increased disposable incomes, and surging interest in natural personal care and healthcare solutions in countries like China, Japan, and India. The convergence of these factors not only underlines propolis's relevance in contemporary health trends but also highlights promising opportunities for stakeholders within this dynamic sector.
+Top-down and bottom-up approaches were used to estimate and validate the size of the Global Propolis market and to estimate the size of various other dependent submarkets. The research methodology used to estimate the market size includes the following details: The key players in the market were identified through secondary research, and their market shares in the respective regions were determined through primary and secondary research. This entire procedure includes the study of the annual and financial reports of the top market players and extensive interviews for key insights from industry leaders such as CEOs, VPs, directors, and marketing executives. All percentage shares split, and breakdowns were determined using secondary sources and verified through Primary sources. All possible parameters that affect the markets covered in this research study have been accounted for, viewed in extensive detail, verified through primary research, and analyzed to get the final quantitative and qualitative data.
+Global Propolis Market Segmental Analysis
+Global Propolis Market is segmented by Product Type, Distribution Channel, and Region. Based on Product Type, the market is segmented into Capsules and Tablets, Liquids, and Others. Based on Distribution Channel, the market is segmented into Retail Store, Online, and Others. Based on region, the market is segmented into North America, Europe, Asia Pacific, Latin America and Middle East &amp; Africa.
+Driver of the Global Propolis Market
+The global propolis market is significantly driven by the rising consumer preference for natural and organic products across diverse sectors such as food and beverage, cosmetics, and healthcare. As awareness of the health benefits associated with propolis increases, consumers are gravitating towards products that incorporate this natural ingredient, leading to heightened demand. Propolis's unique properties as a natural food preservative and flavor enhancer further bolster its appeal in the food and beverage industry. This trend reflects a broader shift toward sustainability and health consciousness, positioning propolis as a sought-after component across multiple consumer markets and catalyzing robust market growth.
+Restraints in the Global Propolis Market
+The global propolis market faces significant restraints primarily due to the limited availability of this natural resin, which is contingent on factors such as climatic conditions, seasonal variations, and specific geographic locations. The ongoing decline in bee populations, driven by environmental concerns and habitat loss, exacerbates supply issues, as bees are vital to propolis production. Additionally, the extraction and processing of propolis involve high costs, further constraining market growth and accessibility. These intertwined factors create a challenging landscape for the propolis market, impeding its expansion and limiting the potential for widespread application and commercialization.
+Market Trends of the Global Propolis Market
+The global propolis market is witnessing significant growth, driven by the escalating demand for propolis-based products in the cosmetics and personal care industries. Recognized for its antibacterial and anti-inflammatory properties, propolis is becoming a sought-after ingredient in natural and organic skincare formulations, reflecting a broader market shift towards clean beauty. Additionally, its incorporation into functional foods and dietary supplements is gaining traction, fueled by a growing consumer awareness of health benefits associated with natural products. This dual demand across multiple sectors is positioning propolis as a key player in the trend towards holistic wellness and sustainable beauty solutions.</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>• Introduction
+o Objectives of the Study
+o Definitions
+o Market Scope
+• Research Methodology
+o Information Procurement
+o Secondary &amp; Primary Data Sources
+o Market Size Estimation
+o Market Assumptions &amp; Limitations
+• Executive Summary
+o Market Overview Outlook
+o Supply Demand Trend Analysis
+o Segmental Opportunity Analysis
+• Market Dynamics &amp; Outlook
+o Market Dynamics
+ Drivers
+ Opportunities
+ Restraints
+ Challenges
+o Porters Analysis
+ Competitive rivalry
+ Threat of Substitute Products
+ Bargaining Power of Buyers
+ Threat of New Entrants
+ Bargaining Power of Suppliers
+• Key Market Insights
+o Key Success Factor
+o Degree of Competition
+o Top Investment Pockets
+o Ecosystem of the Market
+o Technology Analysis
+o Market Entry Strategies
+o Case Study Analysis
+o Customer &amp; Buying Criteria Analysis
+o Regulatory Landscape
+• Propolis Market, By Product Type
+o Market Overview
+o Capsules And Tablets
+o Liquids
+o Others
+• Propolis Market, By Distribution Channel
+o Market Overview
+o Retail Store
+o Online
+o Others
+• Propolis Market Size by Region
+o Market Overview
+o North America
+ USA
+ Canada
+o Europe
+ Germany
+ Spain
+ France
+ UK
+ Italy
+ Rest of Europe
+o Asia Pacific
+ China
+ India
+ Japan
+ South Korea
+ Rest of Asia-Pacific
+o Latin America
+ Brazil
+ Rest of Latin America
+o Middle East &amp; Africa (MEA)
+ GCC Countries
+ South Africa
+ Rest of MEA
+• Competitive Landscape
+o Top 5 Player Comparison
+o Market Positioning of Key Players, 2023
+o Strategies Adopted by Key Market Players
+o Recent Activities in the Market
+o Key Companies Market Share (%), 2023
+• Key Company Profiles
+o Herb Pharm LLC
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Apis Flora
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Bee Health Limited
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o YS Organic Bee Farms
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Comvita Ltd
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Wax Green
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Uniflora Health Food
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Sunyata Pon Lee
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o NOW Foods
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o API Health
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Comvita Limited
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Bee Health Limited
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Wax Green
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o MN Propolis
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Ponlee
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Ponlee Bee
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Sunyata Pon Lee Bee
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Honey Pacifica
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Honey Gardens
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Beekeeper's Naturals
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Beehive Botanicals Inc.
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Durham's Bee Farm
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Y.S. Eco Bee Farms
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o NaturaNectar LLC
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Health Care</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>◦ USA
+◦ Canada
+◦ Germany
+◦ Spain
+◦ Italy
+◦ France
+◦ UK
+◦ China
+◦ India
+◦ Japan
+◦ South Korea
+◦ Brazil
+◦ GCC Countries
+◦ South Africa</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>◦ Herb Pharm LLC
+◦ 
+◦ 
+◦ 
+◦ Apis Flora
+◦ Bee Health Limited
+◦ YS Organic Bee Farms
+◦ Comvita Ltd
+◦ Wax Green
+◦ Uniflora Health Food
+◦ Sunyata Pon Lee
+◦ NOW Foods
+◦ API Health
+◦ Comvita Limited
+◦ Bee Health Limited
+◦ Wax Green
+◦ MN Propolis
+◦ Ponlee
+◦ Ponlee Bee
+◦ Sunyata Pon Lee Bee
+◦ Honey Pacifica
+◦ Honey Gardens
+◦ Beekeeper's Naturals
+◦ Beehive Botanicals Inc.
+◦ Durham's Bee Farm
+◦ Y.S. Eco Bee Farms
+◦ NaturaNectar LLC</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>By Product Type (Capsules and Tablets, Liquids, Others), By Distribution Channel (Retail Store, Online, Others)</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>651.57</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>666.69</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>800.96</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>2.32%</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>USD Million</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Insulin Pump Market Size, Share, Growth Analysis, By Type (Patch Pumps, And Tethered Pumps), By Product (MiniMed, Accu-Chek), By Accessories (Insulin Reservoir or Cartridges, Insulin Set Insertion Devices), By End Use (Hospitals &amp; Clinics, Homecare), By Region - Industry Forecast 2024-2031</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SQMIG35A2135</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.skyquestt.com/report/insulin-pump-market</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>165</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>5300</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>6200</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>7100</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>Global Insulin Pump Market size was valued at USD 5.59 billion in 2022 and is poised to grow from USD 6.05 billion in 2023 to USD 11.38 billion by 2031, growing at a CAGR of 8.22 % in the forecast period (2024-2031).
-The insulin pump market is witnessing substantial growth, driven by the rising global prevalence of diabetes, particularly type 1 diabetes, and the increasing demand for advanced portable insulin delivery systems among patients. This technological innovation is propelled by major medical device manufacturers integrating smart technologies, such as artificial intelligence and machine learning, into insulin pumps. As of 2019, the International Diabetes Federation reported approximately 537 million individuals living with diabetes, a figure projected to surge to 783 million by 2045. This alarming trend underscores the urgent need for effective diabetes management solutions, as untreated diabetes can lead to severe complications like blindness, renal failure, and strokes. Additionally, the insulin pump market is buoyed by factors such as escalating healthcare costs, enhanced access to healthcare services, and the growing availability of cutting-edge insulin delivery devices. The U.S. insulin pump market, in particular, is expected to experience a sustainable compound annual growth rate (CAGR) in the upcoming forecast period, reflecting a robust response to the increasing requirements of diabetic patients seeking convenient and efficient management options. Overall, the insulin pump sector is positioned for significant expansion as awareness, technology, and healthcare infrastructures evolve in tandem to address the burgeoning diabetes epidemic.
+The insulin pump market is experiencing significant growth, driven primarily by the rising global prevalence of diabetes, particularly type 1 diabetes. With over 537 million individuals affected by diabetes in 2019, a number projected to reach 783 million by 2045 according to the International Diabetes Federation (IDF), the demand for portable insulin delivery systems has surged within the diabetic community. This has led to advancements in sophisticated insulin pump technology, integrating innovative features powered by artificial intelligence (AI) and machine learning (ML) from leading medical device manufacturers. These developments cater to the increasing need for effective diabetes management solutions, as diabetes poses risks of severe health complications such as blindness, renal failure, and stroke, as noted by the World Health Organization. Moreover, factors such as rising healthcare costs, improved access to medical facilities, and the growing availability of advanced insulin delivery systems contribute to the thriving market. Specifically, the US insulin pump market is expected to maintain a robust compound annual growth rate (CAGR) in the upcoming forecast period, reflecting a strong demand for these essential devices. As the industry adapts to meet the needs of an expanding demographic struggling with diabetes, the convergence of technology and healthcare continues to shape the future of insulin delivery systems.
 Top-down and bottom-up approaches were used to estimate and validate the size of the Global Insulin Pump market and to estimate the size of various other dependent submarkets. The research methodology used to estimate the market size includes the following details: The key players in the market were identified through secondary research, and their market shares in the respective regions were determined through primary and secondary research. This entire procedure includes the study of the annual and financial reports of the top market players and extensive interviews for key insights from industry leaders such as CEOs, VPs, directors, and marketing executives. All percentage shares split, and breakdowns were determined using secondary sources and verified through Primary sources. All possible parameters that affect the markets covered in this research study have been accounted for, viewed in extensive detail, verified through primary research, and analyzed to get the final quantitative and qualitative data.
 Global Insulin Pump Market Segmental Analysis
 Global Insulin Pump Market is segmented on the basis of type, product, accessories, end use, and region. By type, market is segmented into patch pumps, and tethered pumps. By product, market is segmented into MiniMed, Accu-Chek, Tandem, Omnipod, and others. By accessories, market is segmented into insulin reservoir or cartridges, insulin set insertion devices, and battery. By End use, market is segmented into hospitals &amp; clinics, homecare, and laboratories. By region, the market is segmented into North America, Europe, Asia Pacific, Middle East and Africa, and Latin America.
 Driver of the Global Insulin Pump Market
-The Global Insulin Pump market is significantly driven by the increasing adoption of insulin pumps among diabetic patients, both in developed and emerging economies. Market participants are heavily investing in research and development to create advanced, user-friendly technologies that enhance patient outcomes. With a growing focus on innovative product launches, these companies are responding to the demand for improved diabetes management solutions. Clinical trials highlighting the effectiveness of pump therapy in achieving better glucose control in type 2 diabetes patients, compared to traditional Multiple Daily Injection (MDI) methods, further bolster the market, showcasing the potential of insulin pumps to enhance patient quality of life.
+The global insulin pump market is significantly driven by the increasing adoption of advanced insulin delivery systems among diabetic patients, fueled by continuous research and development (R&amp;D) efforts from market participants. As innovations emerge, including smart insulin pumps equipped with integrated continuous glucose monitoring systems and automated insulin delivery capabilities, the appeal of these devices grows. Clinical trials demonstrating superior glucose control in type 2 diabetes patients utilizing pump therapy over traditional Multiple Daily Injection (MDI) methods further enhance the market's momentum. This trend not only reflects a shift towards more effective diabetes management solutions but also responds to the growing demand for personalized healthcare technologies in both developed and emerging economies.
 Restraints in the Global Insulin Pump Market
-The Global Insulin Pump market faces significant restraints stemming from low reimbursement options and the high cost associated with insulin pumps, which deter patient adoption. Many individuals, particularly those in underdeveloped and emerging countries, rely heavily on insurance reimbursements to access necessary treatments. Furthermore, a lack of awareness and understanding of diabetes management and insulin pumps exacerbates this challenge, as evidenced by the estimated 232 million undiagnosed diabetics worldwide in 2019. The inadequate healthcare infrastructure in these regions hinders patient education and accessibility, ultimately constraining market growth and adoption rates of insulin pump technology.
+The global insulin pump market faces significant restraints, particularly from limited reimbursement options and the high costs associated with these devices. Many patients depend on insurance or government reimbursements to afford diabetes management tools, which can be prohibitively expensive for many individuals. This financial burden results in a reluctance to adopt insulin pumps, subsequently hindering market growth. Furthermore, the awareness and availability of insulin pumps are particularly low in underdeveloped and emerging regions, where healthcare infrastructure is inadequate. With approximately 232 million diabetics undiagnosed as of 2019, the lack of recognition and treatment options poses a critical barrier to market expansion.
 Market Trends of the Global Insulin Pump Market
-The Global Insulin Pump market is witnessing a significant trend towards the integration of intelligent technologies, particularly artificial intelligence (AI), revolutionizing diabetes management. As healthcare IT continues to evolve, medical device manufacturers are increasingly developing AI-enabled insulin pumps and automated drug delivery systems tailored for type 2 diabetes patients. The market is responding to the growing demand for advanced, user-friendly insulin delivery solutions, with current adoption rates for type 2 insulin pumps at approximately 5%. This is projected to expand by 15% by 2027, driven by technological advancements and a rising population managing diabetes, solidifying the relevance of smart devices in chronic disease management.</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
+The Global Insulin Pump market is witnessing a significant upward trend, primarily driven by advancements in intelligent technologies, including artificial intelligence (AI), which are revolutionizing diabetes management. As diabetes cases surge, especially among type 2 diabetes patients, there is an increasing demand for innovative, automated drug delivery systems. Medical device companies are responding to this demand by developing AI-enabled insulin pumps, enhancing both efficacy and user experience. Current statistics indicate a modest global adoption rate of around 5% for type 2 insulin pumps, poised to expand to 15% by 2027, highlighting the market's potential for growth and the shift towards more sophisticated healthcare solutions.</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>• Introduction
 o Objectives of the Study
@@ -785,14 +1126,14 @@
  Key Developments</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
         <is>
           <t>Health Care</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>◦ USA
 ◦ Canada
@@ -810,7 +1151,7 @@
 ◦ South Africa</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>◦ Medtronic (Ireland)
 ◦ 
@@ -838,32 +1179,32 @@
 ◦ Nipro Diagnostic, Inc. (Japan)</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>By Type (Patch pumps, and Tethered pumps), By Product (MiniMed, Accu-Chek, Tandem, Omnipod, and others), By Accessories (Insulin Eeservoir or Cartridges, Insulin Set Insertion Devices, and Battery), By End Use (Hospitals &amp; Clinics, Homecare, and Laboratories)</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>5.59</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>6.05</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>11.38</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>8.22%</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>USD Billion</t>
         </is>

</xml_diff>

<commit_message>
before new wnebsite h2
</commit_message>
<xml_diff>
--- a/GII.xlsx
+++ b/GII.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -40,6 +40,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
         <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -55,9 +61,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -547,59 +554,49 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Endodontic Devices Market Size, Share, Growth Analysis, By Product (Instruments, Consumables), By End-User (Dental Clinics, Hospitals), By Region - Industry Forecast 2025-2032</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>SQSG35A2096</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://www.skyquestt.com/report/endodontic-devices-market</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>242</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Technical Ceramics Market Size, Share, Growth Analysis, By Raw Material (Alumina Ceramics, Titanate Ceramics), By Product (Monolithic ceramics, Ceramic coatings), By Application, By End-use, By Region - Industry Forecast 2025-2032</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>SQMIG15E2424</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>https://www.skyquestt.com/report/technical-ceramics-market</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>157</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr"/>
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>5300</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>6200</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>7100</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Global Endodontic Devices Market size was valued at USD 1.98 billion in 2023 and is poised to grow from USD 2.08 billion in 2024 to USD 3.02 billion by 2032, growing at a CAGR of 4.8% during the forecast period (2025-2032).
-The global market for endodontic devices is set for significant growth, driven by advancements in dental technology and increasing patient preferences for high-quality surgical treatments at dental hospitals. Electric motor dental units, favored for their high torque and cost-effectiveness compared to air-driven units, enhance the efficiency of root canal procedures. Demand for apex locators is particularly robust, fueled by a rise in dental care facilities, prevalence of periodontal diseases, and a surge in dental tourism, alongside heightened awareness of oral hygiene. These modern electronic devices, boasting over 90% accuracy in locating the apical major foramen, are integral to effective treatment planning, further propelling market growth as dental clinics emphasize personalized care and technological upgrades.
-Top-down and bottom-up approaches were used to estimate and validate the size of the Global Endodontic Devices market and to estimate the size of various other dependent submarkets. The research methodology used to estimate the market size includes the following details: The key players in the market were identified through secondary research, and their market shares in the respective regions were determined through primary and secondary research. This entire procedure includes the study of the annual and financial reports of the top market players and extensive interviews for key insights from industry leaders such as CEOs, VPs, directors, and marketing executives. All percentage shares split, and breakdowns were determined using secondary sources and verified through Primary sources. All possible parameters that affect the markets covered in this research study have been accounted for, viewed in extensive detail, verified through primary research, and analyzed to get the final quantitative and qualitative data.
-Global Endodontic Devices Market Segmental Analysis
-Global Endodontic Devices Market is segmented by Component, End-User and region. Based on Component, the market is segmented into Instruments and Consumables. Based on End-User, the market is segmented into Dental Clinics, Hospitals and Dental Academic and Research Institutes. Based on region, the market is segmented into North America, Europe, Asia Pacific, Latin America and Middle East &amp; Africa.
-Driver of the Global Endodontic Devices Market
-The growth of the global endodontic devices market is significantly driven by the rising awareness surrounding oral hygiene and overall well-being. With the influence of social media and celebrities, more individuals are becoming conscious of dental aesthetics and are seeking dental procedures to achieve perfect teeth. This shift in mindset contrasts sharply with previous attitudes, where dental care was often overlooked. Additionally, the demand for personalized endodontic solutions has spurred the adoption of CAD technologies, while cone-beam computed tomography (CT) systems enable dentists to produce detailed 3D images for improved treatment planning. As dental care expenditures rise and tooth decay cases become more prevalent, the market for obturation devices is also projected to grow rapidly.
-Restraints in the Global Endodontic Devices Market
-The Global Endodontic Devices market is currently facing significant challenges that may hinder its growth. One of the primary restraints is the increase in oral infections linked to the use of these devices. Issues such as operational failures of rotary instruments, surgical trauma, complications like apicectomies, ecchymosis, paraesthesia, maxillary sinusitis, and extended gum bleeding are contributing to this concern. These adverse effects not only affect patient outcomes but also lead to hesitancy among dental professionals in adopting these technologies, thereby obstructing the overall advancement and expansion of the market. Addressing these complications will be crucial for future growth.
-Market Trends of the Global Endodontic Devices Market
-The global endodontic devices market is poised for significant growth, driven by escalating dental tourism, advancements in healthcare infrastructure, and favorable reimbursement policies across regions. The rising trend of patients seeking affordable dental care in Asia-Pacific countries, particularly India and China, is a key factor, as these locations offer treatment costs that are 60% to 70% lower than in developed nations. This influx of dental tourists capitalizes on the high number of qualified dental professionals in these regions. As patients increasingly seek value and quality in dental procedures, the endodontic devices market is likely to flourish, reflecting changing global healthcare dynamics.</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>Report details not available.</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>• Introduction
 o Objectives of the Study
@@ -636,56 +633,66 @@
 o Macro-Economic Indicators
 o Value Chain Analysis
 o Pricing Analysis
-o Case Studies
-o Technology Advancement
-o Regulatory Landscape
+o Raw Material Analysis
+o Technology Analysis
 o Patent Analysis
-o Trade Analysis
-• Global Endodontic Devices Market Size by Component &amp; CAGR (2025-2032)
+o Raw Material Analysis
+• Global Technical Ceramics Market Size by Raw Material &amp; CAGR (2025-2032)
 o Market Overview
-o Instruments
- Endodontic Motors
- Apex Locators
- Endodontic Scalers
- Endodontic Handpieces
-o Consumables
- Endodontic Files
- Stainless Steel Files
- Nickel-Titanium (NiTi) Files
- Endodontic Burs
- Endodontic Irrigating Solutions
- Endodontic Obturation Materials
- Gutta-Percha
- Sealers
- Others
- Lubricants
- Medicaments
-• Global Endodontic Devices Market Size by End-User &amp; CAGR (2025-2032)
+o Alumina Ceramics
+o Titanate Ceramics
+o Zirconate Ceramics
+o Ferrite Ceramics
+o Aluminium Nitride
+o Silicon Carbide
+o Silicon Nitride
+o Others
+• Global Technical Ceramics Market Size by Product &amp; CAGR (2025-2032)
 o Market Overview
-o Dental Clinics
-o Hospitals
-o Dental Academic and Research Institutes
-• Global Endodontic Devices Market Size &amp; CAGR (2025-2032)
-o North America (Component, End-User)
+o Monolithic ceramics
+o Ceramic coatings
+o Ceramic matrix composites
+o Others
+• Global Technical Ceramics Market Size by Application &amp; CAGR (2025-2032)
+o Market Overview
+o Electrical equipment
+o Catalyst supports
+o Electronic devices
+o Wear parts
+o Engine parts
+o Filters
+o Bioceramics
+o Others
+• Global Technical Ceramics Market Size by End-use &amp; CAGR (2025-2032)
+o Market Overview
+o Electrical &amp; Electronics
+o Automotive
+o Machinery
+o Environmental
+o Medical
+o Military &amp; Defense
+o Others
+• Global Technical Ceramics Market Size &amp; CAGR (2025-2032)
+o North America (Raw Material, Product, Application, End-use)
  US
  Canada
-o Europe (Component, End-User)
+o Europe (Raw Material, Product, Application, End-use)
  Germany
  Spain
  France
  UK
  Italy
  Rest of Europe
-o Asia Pacific (Component, End-User)
+o Asia Pacific (Raw Material, Product, Application, End-use)
  China
  India
  Japan
  South Korea
  Rest of Asia-Pacific
-o Latin America (Component, End-User)
+o Latin America (Raw Material, Product, Application, End-use)
  Brazil
  Rest of Latin America
-o Middle East &amp; Africa (Component, End-User)
+o Middle East &amp; Africa (Raw Material, Product, Application, End-use)
  GCC Countries
  South Africa
  Rest of Middle East &amp; Africa
@@ -701,77 +708,102 @@
  Company's Segmental Share Analysis
  Revenue Y-O-Y Comparison (2022-2024)
 • Key Company Profiles
-o Danaher Corporation (USA)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Dentsply Sirona Inc. (USA)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o COLTENE Holding AG (Switzerland)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Ivoclar Vivadent AG (Liechtenstein)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Septodont Holding (France)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Ultradent Products Inc. (USA)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Brasseler USA (USA)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o FKG Dentaire SA (Switzerland)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o DiaDent Group International (South Korea)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Micro-Mega SA (France)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Kerr Corporation (USA)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Henry Schein, Inc. (USA)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o 3M Company (USA)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Shenzhen Perfect Medical Instruments Co., Ltd. (China)
- Company Overview
- Business Segment Overview
- Financial Updates
- Key Developments
-o Pac-Dent, Inc. (USA)
+o Kyocera Corporation (Japan)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Morgan Advanced Materials plc (United Kingdom)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Schott AG (Germany)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o CeramTec GmbH (Germany)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o CoorsTek, Inc. (United States)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o NGK Insulators Ltd. (Japan)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o 3M Company (United States)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Saint-Gobain S.A. (France)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Rauschert GmbH (Germany)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Murata Manufacturing Co., Ltd. (Japan)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Corning Incorporated (United States)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o McDanel Advanced Ceramic Technologies LLC (United States)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Ceradyne, Inc. (United States)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Superior Technical Ceramics Corp. (United States)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Krosaki Harima Corporation (Japan)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o IBIDEN Co., Ltd. (Japan)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o L3Harris Technologies, Inc. (United States)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o RHI Magnesita N.V. (Austria)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Vesuvius plc (United Kingdom)
+ Company Overview
+ Business Segment Overview
+ Financial Updates
+ Key Developments
+o Sumitomo Electric Industries, Ltd. (Japan)
  Company Overview
  Business Segment Overview
  Financial Updates
@@ -779,14 +811,14 @@
 • Conclusion &amp; Recommendations</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Health Care</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
+      <c r="L2" s="2" t="inlineStr"/>
+      <c r="M2" s="2" t="inlineStr"/>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
         <is>
           <t>◦ USA
 ◦ Canada
@@ -804,51 +836,56 @@
 ◦ South Africa</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>◦ Danaher Corporation (USA)
-◦ Dentsply Sirona Inc. (USA)
-◦ COLTENE Holding AG (Switzerland)
-◦ Ivoclar Vivadent AG (Liechtenstein)
-◦ Septodont Holding (France)
-◦ Ultradent Products Inc. (USA)
-◦ Brasseler USA (USA)
-◦ FKG Dentaire SA (Switzerland)
-◦ DiaDent Group International (South Korea)
-◦ Micro-Mega SA (France)
-◦ Kerr Corporation (USA)
-◦ Henry Schein, Inc. (USA)
-◦ 3M Company (USA)
-◦ Shenzhen Perfect Medical Instruments Co., Ltd. (China)
-◦ Pac-Dent, Inc. (USA)</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>By Component (Instruments (Endodontic Motors, Apex Locators, Endodontic Scalers, Endodontic Handpieces), Consumables (Endodontic Files, Endodontic Burs, Endodontic Irrigating Solutions, Endodontic Obturation Materials, Others)), By End-User (Dental Clinics, Hospitals, Dental Academic and Research Institutes)</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>1.98</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>2.08</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>3.02</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>4.8%</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
+      <c r="P2" s="2" t="inlineStr">
+        <is>
+          <t>◦ Kyocera Corporation (Japan)
+◦ Morgan Advanced Materials plc (United Kingdom)
+◦ Schott AG (Germany)
+◦ CeramTec GmbH (Germany)
+◦ CoorsTek, Inc. (United States)
+◦ NGK Insulators Ltd. (Japan)
+◦ 3M Company (United States)
+◦ Saint-Gobain S.A. (France)
+◦ Rauschert GmbH (Germany)
+◦ Murata Manufacturing Co., Ltd. (Japan)
+◦ Corning Incorporated (United States)
+◦ McDanel Advanced Ceramic Technologies LLC (United States)
+◦ Ceradyne, Inc. (United States)
+◦ Superior Technical Ceramics Corp. (United States)
+◦ Krosaki Harima Corporation (Japan)
+◦ IBIDEN Co., Ltd. (Japan)
+◦ L3Harris Technologies, Inc. (United States)
+◦ RHI Magnesita N.V. (Austria)
+◦ Vesuvius plc (United Kingdom)
+◦ Sumitomo Electric Industries, Ltd. (Japan)</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="inlineStr">
+        <is>
+          <t>By Raw Material (Alumina Ceramics, Titanate Ceramics, Zirconate Ceramics, Ferrite Ceramics, Aluminium Nitride, Silicon Carbide, Silicon Nitride, Others), By Product (Monolithic ceramics, Ceramic coatings, Ceramic matrix composites, Others), By Application (Electrical equipment, Catalyst supports, Electronic devices, Wear parts, Engine parts, Filters, Bioceramics, Others), By End-use (Electrical &amp; Electronics, Automotive, Machinery, Environmental, Medical, Military &amp; Defense, Others)</t>
+        </is>
+      </c>
+      <c r="R2" s="2" t="inlineStr">
+        <is>
+          <t>5.89</t>
+        </is>
+      </c>
+      <c r="S2" s="2" t="inlineStr">
+        <is>
+          <t>6.27</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="inlineStr">
+        <is>
+          <t>10.29</t>
+        </is>
+      </c>
+      <c r="U2" s="2" t="inlineStr">
+        <is>
+          <t>6.4%</t>
+        </is>
+      </c>
+      <c r="V2" s="2" t="inlineStr">
         <is>
           <t>USD Billion</t>
         </is>

</xml_diff>